<commit_message>
added stack models, second EDA and candidate end product. Achieved 79% cross validated performance on single model, ensemble and boosting models still not sorted out by idiosincracies in tidymodels stack package.
</commit_message>
<xml_diff>
--- a/calibration_tests/extreme_cases_commented.xlsx
+++ b/calibration_tests/extreme_cases_commented.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubenmontenegro/Library/Mobile Documents/com~apple~CloudDocs/Classtech/Chat Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\RubenMontenegro\Classtech_prototype\Classtech_prototype\calibration_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FB26221-4BDA-9946-A6D2-386623EC25FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B84C44-FE05-4FEF-9F61-92A8020E6DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28120" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extreme_cases" sheetId="1" r:id="rId1"/>
@@ -174,9 +174,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,7 +320,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -812,7 +827,7 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -855,7 +870,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -866,21 +881,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -890,10 +896,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="33" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="18" fillId="33" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -902,7 +905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="33" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="16" fillId="33" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -911,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="33" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="16" fillId="33" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -920,7 +923,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="33" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="16" fillId="33" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -929,7 +932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="16" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -944,7 +947,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1305,1013 +1323,1013 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="76.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13" style="23" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="29" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.5" style="2"/>
+    <col min="2" max="2" width="95.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13" style="19" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="25" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="21" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="26">
+      <c r="C2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="22">
         <v>16</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="22">
         <v>19</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="12">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27">
+      <c r="C3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="23">
         <v>7</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="23">
         <v>19</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="15">
         <v>4.6018387305144</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="27">
+      <c r="C4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="23">
         <v>6</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="23">
         <v>19</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="15">
         <v>4.5462406251802898</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="G4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="27">
+      <c r="C5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23">
         <v>7</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="23">
         <v>18</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="15">
         <v>4.5018387305144003</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="G5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="23">
         <v>19</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="23">
         <v>24</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="15">
         <v>5.4619818783609002</v>
       </c>
-      <c r="G6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="28"/>
+    </row>
+    <row r="7" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="27">
+      <c r="C7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23">
         <v>8</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="23">
         <v>17</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="15">
         <v>4.45</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="27">
+      <c r="C8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="23">
         <v>8</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="23">
         <v>17</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="15">
         <v>4.45</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="27">
+      <c r="C9" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="23">
         <v>8</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="23">
         <v>17</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="15">
         <v>4.45</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="G9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="27">
+      <c r="C10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="23">
         <v>7</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="23">
         <v>17</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="15">
         <v>4.4018387305143998</v>
       </c>
-      <c r="G10" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="G10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="27">
+      <c r="C11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="23">
         <v>6</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="23">
         <v>17</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="15">
         <v>4.3462406251802896</v>
       </c>
-      <c r="G11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="27">
+      <c r="C12" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="23">
         <v>10</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="23">
         <v>15</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="15">
         <v>4.3304820237218404</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="28"/>
+    </row>
+    <row r="13" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="27">
+      <c r="C13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="23">
         <v>7</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="23">
         <v>16</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="15">
         <v>4.3018387305144001</v>
       </c>
-      <c r="G13" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G13" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="14" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="27">
+      <c r="C14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="23">
         <v>9</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="23">
         <v>15</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="15">
         <v>4.2924812503605798</v>
       </c>
-      <c r="G14" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G14" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="28"/>
+    </row>
+    <row r="15" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="27">
+      <c r="C15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="23">
         <v>9</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="23">
         <v>15</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="15">
         <v>4.2924812503605798</v>
       </c>
-      <c r="G15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="28"/>
+    </row>
+    <row r="16" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="27">
+      <c r="C16" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="23">
         <v>9</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="23">
         <v>15</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="15">
         <v>4.2924812503605798</v>
       </c>
-      <c r="G16" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="28"/>
+    </row>
+    <row r="17" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="23">
         <v>14</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="23">
         <v>23</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="15">
         <v>5.2518387305144003</v>
       </c>
-      <c r="G17" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+    <row r="18" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
         <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="27">
+      <c r="C18" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="23">
         <v>6</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="23">
         <v>16</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="15">
         <v>4.24624062518029</v>
       </c>
-      <c r="G18" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="28"/>
+    </row>
+    <row r="19" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
         <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="27">
-        <v>1</v>
-      </c>
-      <c r="E19" s="27">
+      <c r="D19" s="23">
+        <v>1</v>
+      </c>
+      <c r="E19" s="23">
         <v>42</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="15">
         <v>5.2</v>
       </c>
-      <c r="G19" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="G19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="27">
+      <c r="C20" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="23">
         <v>5</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="23">
         <v>16</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="15">
         <v>4.1804820237218401</v>
       </c>
-      <c r="G20" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
         <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="27">
+      <c r="C21" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="23">
         <v>5</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="23">
         <v>16</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="15">
         <v>4.1804820237218401</v>
       </c>
-      <c r="G21" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="28"/>
+    </row>
+    <row r="22" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
         <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="27">
+      <c r="C22" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="23">
         <v>5</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="23">
         <v>16</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="15">
         <v>4.1804820237218401</v>
       </c>
-      <c r="G22" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="28"/>
+    </row>
+    <row r="23" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
         <v>27</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="27">
+      <c r="C23" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="23">
         <v>5</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="23">
         <v>16</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="15">
         <v>4.1804820237218401</v>
       </c>
-      <c r="G23" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="30" t="s">
+      <c r="G23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
         <v>29</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="27">
+      <c r="C24" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="23">
         <v>5</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="23">
         <v>16</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="15">
         <v>4.1804820237218401</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="30" t="s">
+      <c r="G24" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
         <v>30</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="23">
         <v>15</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="23">
         <v>22</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="15">
         <v>5.1767226489021301</v>
       </c>
-      <c r="G25" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="30" t="s">
+      <c r="G25" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
         <v>32</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="27">
+      <c r="C26" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="23">
         <v>6</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="23">
         <v>15</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="15">
         <v>4.1462406251802904</v>
       </c>
-      <c r="G26" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G26" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="28"/>
+    </row>
+    <row r="27" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2">
         <v>33</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="27">
+      <c r="C27" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="23">
         <v>6</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="23">
         <v>15</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="15">
         <v>4.1462406251802904</v>
       </c>
-      <c r="G27" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="28"/>
+    </row>
+    <row r="28" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
         <v>34</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="27">
+      <c r="C28" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="23">
         <v>6</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="23">
         <v>15</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="15">
         <v>4.1462406251802904</v>
       </c>
-      <c r="G28" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G28" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="28"/>
+    </row>
+    <row r="29" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2">
         <v>35</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="27">
+      <c r="C29" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="23">
         <v>6</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="23">
         <v>15</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="15">
         <v>4.1462406251802904</v>
       </c>
-      <c r="G29" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G29" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="28"/>
+    </row>
+    <row r="30" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
         <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="27">
+      <c r="C30" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="23">
         <v>6</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="23">
         <v>15</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="15">
         <v>4.1462406251802904</v>
       </c>
-      <c r="G30" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G30" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="28"/>
+    </row>
+    <row r="31" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
         <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="23">
         <v>13</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E31" s="23">
         <v>22</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="15">
         <v>5.1251099295352702</v>
       </c>
-      <c r="G31" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G31" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" s="28"/>
+    </row>
+    <row r="32" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="2">
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="27">
+      <c r="C32" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="23">
         <v>7</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="23">
         <v>14</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="15">
         <v>4.1018387305144</v>
       </c>
-      <c r="G32" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H32" s="30" t="s">
+      <c r="G32" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
         <v>40</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="27">
+      <c r="C33" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="23">
         <v>4</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="23">
         <v>16</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="15">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G33" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G33" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="28"/>
+    </row>
+    <row r="34" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2">
         <v>41</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D34" s="23">
         <v>12</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="23">
         <v>22</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="15">
         <v>5.0962406251802896</v>
       </c>
-      <c r="G34" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="28"/>
+    </row>
+    <row r="35" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2">
         <v>43</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="27">
+      <c r="C35" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="23">
         <v>5</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="23">
         <v>15</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="15">
         <v>4.0804820237218404</v>
       </c>
-      <c r="G35" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H35" s="30" t="s">
+      <c r="G35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2">
         <v>44</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="27">
+      <c r="C36" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="23">
         <v>5</v>
       </c>
-      <c r="E36" s="27">
+      <c r="E36" s="23">
         <v>15</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F36" s="15">
         <v>4.0804820237218404</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H36" s="30" t="s">
+      <c r="G36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="29" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
         <v>46</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="27">
+      <c r="C37" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="23">
         <v>6</v>
       </c>
-      <c r="E37" s="27">
+      <c r="E37" s="23">
         <v>14</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="15">
         <v>4.0462406251802898</v>
       </c>
-      <c r="G37" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G37" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2">
         <v>47</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="27">
+      <c r="C38" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="23">
         <v>7</v>
       </c>
-      <c r="E38" s="27">
+      <c r="E38" s="23">
         <v>13</v>
       </c>
-      <c r="F38" s="19">
+      <c r="F38" s="15">
         <v>4.0018387305144003</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G38" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" s="28"/>
+    </row>
+    <row r="39" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
         <v>48</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="27">
+      <c r="C39" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="23">
         <v>7</v>
       </c>
-      <c r="E39" s="27">
+      <c r="E39" s="23">
         <v>13</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="15">
         <v>4.0018387305144003</v>
       </c>
-      <c r="G39" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="28"/>
+    </row>
+    <row r="40" spans="1:8" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>50</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="28">
+      <c r="C40" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="24">
         <v>4</v>
       </c>
-      <c r="E40" s="28">
+      <c r="E40" s="24">
         <v>15</v>
       </c>
-      <c r="F40" s="22">
+      <c r="F40" s="18">
         <v>4</v>
       </c>
-      <c r="G40" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H40" s="6"/>
+      <c r="G40" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>